<commit_message>
Update source SIT for ROM.
</commit_message>
<xml_diff>
--- a/sits/msit_rom.xlsx
+++ b/sits/msit_rom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="929" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -171,7 +171,7 @@
     <t>Heavy Variant</t>
   </si>
   <si>
-    <t>PHX (SCS)</t>
+    <t>PHX</t>
   </si>
   <si>
     <t>13P(6)/7P(3)</t>
@@ -2293,16 +2293,16 @@
     <t>Pioneer Eagle, Survey Ship, Scout, EW=2; Carry 2EP if not surveying.</t>
   </si>
   <si>
-    <t>FE (3FE)</t>
-  </si>
-  <si>
-    <t>6-18T/3-9</t>
-  </si>
-  <si>
-    <t>From 3xWE/KE: 3</t>
-  </si>
-  <si>
-    <t>Tug (Special Limits) Unbreakable.</t>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>2-6U/1-3</t>
+  </si>
+  <si>
+    <t>From WE/KE: 3</t>
+  </si>
+  <si>
+    <t>Theater Transport</t>
   </si>
   <si>
     <t>CE</t>
@@ -4026,12 +4026,6 @@
       <sz val="9"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="9"/>
-    </font>
-    <font>
       <name val="Times New Roman"/>
       <charset val="204"/>
       <family val="1"/>
@@ -4056,6 +4050,12 @@
       <name val="MS Gothic"/>
       <charset val="1"/>
       <family val="3"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="9"/>
     </font>
   </fonts>
@@ -4100,10 +4100,10 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
       <diagonal/>
     </border>
   </borders>
@@ -4132,7 +4132,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -4141,11 +4141,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4153,7 +4153,7 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="7" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4165,11 +4165,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4177,11 +4177,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4189,11 +4189,11 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="167" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4209,11 +4209,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4221,23 +4221,19 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="167" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="167" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4245,15 +4241,11 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="166" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4261,19 +4253,19 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="166" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="166" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4305,27 +4297,23 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="167" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="168" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="168" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="8" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="7" numFmtId="168" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="8" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="7" numFmtId="168" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -4412,8 +4400,8 @@
   </sheetPr>
   <dimension ref="A1:K230"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A198" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A202" activeCellId="0" pane="topLeft" sqref="202:203"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E18" activeCellId="0" pane="topLeft" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4709,13 +4697,13 @@
       <c r="G10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="J10" s="26" t="n">
+      <c r="J10" s="25" t="n">
         <v>4.25</v>
       </c>
       <c r="K10" s="18" t="s">
@@ -4726,7 +4714,7 @@
       <c r="A11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -4835,7 +4823,7 @@
       <c r="I14" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J14" s="28" t="n">
+      <c r="J14" s="27" t="n">
         <v>3.5</v>
       </c>
       <c r="K14" s="10" t="s">
@@ -4885,7 +4873,7 @@
       <c r="I16" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J16" s="28" t="n">
+      <c r="J16" s="27" t="n">
         <v>5</v>
       </c>
       <c r="K16" s="10" t="s">
@@ -4920,7 +4908,7 @@
       <c r="I17" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="J17" s="29" t="n">
+      <c r="J17" s="28" t="n">
         <v>5</v>
       </c>
       <c r="K17" s="16" t="s">
@@ -4955,7 +4943,7 @@
       <c r="I18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="28" t="n">
+      <c r="J18" s="27" t="n">
         <v>4</v>
       </c>
       <c r="K18" s="10" t="s">
@@ -4999,10 +4987,10 @@
       <c r="G20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="10" t="s">
         <v>97</v>
       </c>
       <c r="J20" s="11" t="n">
@@ -5019,7 +5007,7 @@
       <c r="B21" s="8" t="n">
         <v>72</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="26" t="s">
         <v>100</v>
       </c>
       <c r="D21" s="7" t="s">
@@ -5048,37 +5036,37 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="22">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="32" t="n">
+      <c r="B22" s="30" t="n">
         <v>29</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="33" t="n">
+      <c r="E22" s="31" t="n">
         <v>9</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="10" t="s">
         <v>107</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="34" t="n">
+      <c r="J22" s="32" t="n">
         <v>2.5</v>
       </c>
-      <c r="K22" s="31" t="s">
+      <c r="K22" s="29" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5139,13 +5127,13 @@
       <c r="G24" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="16" t="s">
         <v>116</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J24" s="35" t="n">
+      <c r="J24" s="33" t="n">
         <v>2.5</v>
       </c>
       <c r="K24" s="18" t="s">
@@ -5174,13 +5162,13 @@
       <c r="G25" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="16" t="s">
         <v>123</v>
       </c>
       <c r="I25" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="J25" s="26" t="n">
+      <c r="J25" s="25" t="n">
         <v>2</v>
       </c>
       <c r="K25" s="18" t="s">
@@ -5244,13 +5232,13 @@
       <c r="G27" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="H27" s="16" t="s">
         <v>129</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="J27" s="35" t="n">
+      <c r="J27" s="33" t="n">
         <v>2.5</v>
       </c>
       <c r="K27" s="18" t="s">
@@ -5264,7 +5252,7 @@
       <c r="B28" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="34" t="s">
         <v>133</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -5279,7 +5267,7 @@
       <c r="G28" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="H28" s="10" t="s">
         <v>134</v>
       </c>
       <c r="I28" s="10" t="s">
@@ -5296,10 +5284,10 @@
       <c r="A29" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="34" t="s">
         <v>138</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -5358,7 +5346,7 @@
       <c r="J30" s="11" t="n">
         <v>2.5</v>
       </c>
-      <c r="K30" s="30" t="s">
+      <c r="K30" s="10" t="s">
         <v>144</v>
       </c>
     </row>
@@ -5405,7 +5393,7 @@
       <c r="I32" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="J32" s="28" t="n">
+      <c r="J32" s="27" t="n">
         <v>2</v>
       </c>
       <c r="K32" s="10" t="s">
@@ -5475,7 +5463,7 @@
       <c r="I34" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="J34" s="28" t="n">
+      <c r="J34" s="27" t="n">
         <v>2</v>
       </c>
       <c r="K34" s="10" t="s">
@@ -5504,13 +5492,13 @@
       <c r="G35" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="16" t="s">
         <v>165</v>
       </c>
       <c r="I35" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="J35" s="26" t="n">
+      <c r="J35" s="25" t="n">
         <v>2</v>
       </c>
       <c r="K35" s="16" t="s">
@@ -5539,13 +5527,13 @@
       <c r="G36" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="16" t="s">
         <v>170</v>
       </c>
       <c r="I36" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="J36" s="35" t="n">
+      <c r="J36" s="33" t="n">
         <v>2</v>
       </c>
       <c r="K36" s="18" t="s">
@@ -5553,34 +5541,34 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="43" outlineLevel="0" r="37">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="32" t="n">
+      <c r="B37" s="30" t="n">
         <v>109</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="E37" s="33" t="n">
+      <c r="E37" s="31" t="n">
         <v>8</v>
       </c>
-      <c r="F37" s="31" t="s">
+      <c r="F37" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="H37" s="30" t="s">
+      <c r="H37" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="I37" s="31" t="s">
+      <c r="I37" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J37" s="34" t="n">
+      <c r="J37" s="32" t="n">
         <v>2</v>
       </c>
       <c r="K37" s="7" t="s">
@@ -5594,7 +5582,7 @@
       <c r="B38" s="8" t="n">
         <v>75</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="36" t="s">
         <v>177</v>
       </c>
       <c r="D38" s="7" t="s">
@@ -5629,7 +5617,7 @@
       <c r="B39" s="24" t="n">
         <v>113</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="37" t="s">
         <v>181</v>
       </c>
       <c r="D39" s="18" t="s">
@@ -5650,7 +5638,7 @@
       <c r="I39" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J39" s="35" t="n">
+      <c r="J39" s="33" t="n">
         <v>2</v>
       </c>
       <c r="K39" s="16" t="s">
@@ -5664,7 +5652,7 @@
       <c r="B40" s="24" t="n">
         <v>130</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="38" t="s">
         <v>185</v>
       </c>
       <c r="D40" s="18" t="s">
@@ -5679,13 +5667,13 @@
       <c r="G40" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="H40" s="25" t="s">
+      <c r="H40" s="16" t="s">
         <v>186</v>
       </c>
       <c r="I40" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="J40" s="35" t="n">
+      <c r="J40" s="33" t="n">
         <v>2</v>
       </c>
       <c r="K40" s="18" t="s">
@@ -5699,7 +5687,7 @@
       <c r="B41" s="8" t="n">
         <v>121</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="34" t="s">
         <v>190</v>
       </c>
       <c r="D41" s="7" t="s">
@@ -5734,7 +5722,7 @@
       <c r="B42" s="8" t="n">
         <v>108</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="35" t="s">
         <v>196</v>
       </c>
       <c r="D42" s="7" t="s">
@@ -5749,7 +5737,7 @@
       <c r="G42" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="10" t="s">
         <v>197</v>
       </c>
       <c r="I42" s="7" t="s">
@@ -5758,7 +5746,7 @@
       <c r="J42" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="K42" s="30" t="s">
+      <c r="K42" s="10" t="s">
         <v>199</v>
       </c>
     </row>
@@ -5790,7 +5778,7 @@
       <c r="I43" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="J43" s="28" t="n">
+      <c r="J43" s="27" t="n">
         <v>3.5</v>
       </c>
       <c r="K43" s="10" t="s">
@@ -5886,7 +5874,7 @@
       <c r="A47" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="26" t="s">
         <v>37</v>
       </c>
       <c r="C47" s="10" t="s">
@@ -5959,7 +5947,7 @@
       <c r="B49" s="24" t="n">
         <v>16</v>
       </c>
-      <c r="C49" s="41" t="s">
+      <c r="C49" s="39" t="s">
         <v>220</v>
       </c>
       <c r="D49" s="18" t="s">
@@ -5980,7 +5968,7 @@
       <c r="I49" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="J49" s="26" t="n">
+      <c r="J49" s="25" t="n">
         <v>1.25</v>
       </c>
       <c r="K49" s="18" t="s">
@@ -5994,7 +5982,7 @@
       <c r="B50" s="20" t="n">
         <v>19</v>
       </c>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="40" t="s">
         <v>225</v>
       </c>
       <c r="D50" s="16" t="s">
@@ -6099,7 +6087,7 @@
       <c r="B53" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="C53" s="34" t="s">
         <v>220</v>
       </c>
       <c r="D53" s="7" t="s">
@@ -6114,13 +6102,13 @@
       <c r="G53" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="H53" s="10" t="s">
         <v>237</v>
       </c>
       <c r="I53" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="J53" s="43" t="n">
+      <c r="J53" s="41" t="n">
         <v>1.25</v>
       </c>
       <c r="K53" s="10" t="s">
@@ -6134,7 +6122,7 @@
       <c r="B54" s="15" t="n">
         <v>70</v>
       </c>
-      <c r="C54" s="38" t="s">
+      <c r="C54" s="36" t="s">
         <v>241</v>
       </c>
       <c r="D54" s="10" t="s">
@@ -6190,10 +6178,10 @@
       <c r="I55" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="J55" s="26" t="n">
+      <c r="J55" s="25" t="n">
         <v>1.25</v>
       </c>
-      <c r="K55" s="25" t="s">
+      <c r="K55" s="16" t="s">
         <v>247</v>
       </c>
     </row>
@@ -6204,7 +6192,7 @@
       <c r="B56" s="24" t="n">
         <v>103</v>
       </c>
-      <c r="C56" s="41" t="s">
+      <c r="C56" s="39" t="s">
         <v>249</v>
       </c>
       <c r="D56" s="18" t="s">
@@ -6225,7 +6213,7 @@
       <c r="I56" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="J56" s="26" t="n">
+      <c r="J56" s="25" t="n">
         <v>1.25</v>
       </c>
       <c r="K56" s="16" t="s">
@@ -6274,7 +6262,7 @@
       <c r="B58" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="C58" s="36" t="s">
+      <c r="C58" s="34" t="s">
         <v>260</v>
       </c>
       <c r="D58" s="7" t="s">
@@ -6295,7 +6283,7 @@
       <c r="I58" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="J58" s="43" t="n">
+      <c r="J58" s="41" t="n">
         <v>1.25</v>
       </c>
       <c r="K58" s="10" t="s">
@@ -6330,7 +6318,7 @@
       <c r="I59" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="J59" s="28" t="n">
+      <c r="J59" s="27" t="n">
         <v>3</v>
       </c>
       <c r="K59" s="10" t="s">
@@ -6380,7 +6368,7 @@
       <c r="I61" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="J61" s="43" t="n">
+      <c r="J61" s="41" t="n">
         <v>1.25</v>
       </c>
       <c r="K61" s="10" t="s">
@@ -6394,7 +6382,7 @@
       <c r="B62" s="20" t="n">
         <v>89</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="39" t="s">
         <v>277</v>
       </c>
       <c r="D62" s="16" t="s">
@@ -6500,7 +6488,7 @@
       <c r="I65" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="J65" s="44" t="n">
+      <c r="J65" s="42" t="n">
         <v>0.875</v>
       </c>
       <c r="K65" s="10" t="s">
@@ -6514,7 +6502,7 @@
       <c r="B66" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C66" s="36" t="s">
+      <c r="C66" s="34" t="s">
         <v>293</v>
       </c>
       <c r="D66" s="7" t="s">
@@ -6529,13 +6517,13 @@
       <c r="G66" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="H66" s="30" t="s">
+      <c r="H66" s="10" t="s">
         <v>294</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="J66" s="43" t="n">
+      <c r="J66" s="41" t="n">
         <v>0.88</v>
       </c>
       <c r="K66" s="10" t="s">
@@ -6546,7 +6534,7 @@
       <c r="A67" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="B67" s="27" t="s">
+      <c r="B67" s="26" t="s">
         <v>37</v>
       </c>
       <c r="C67" s="10" t="s">
@@ -6605,7 +6593,7 @@
       <c r="I68" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="J68" s="45" t="n">
+      <c r="J68" s="43" t="n">
         <v>0.875</v>
       </c>
       <c r="K68" s="16" t="s">
@@ -6619,7 +6607,7 @@
       <c r="B69" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="C69" s="42" t="s">
+      <c r="C69" s="40" t="s">
         <v>306</v>
       </c>
       <c r="D69" s="16" t="s">
@@ -6640,7 +6628,7 @@
       <c r="I69" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="J69" s="45" t="n">
+      <c r="J69" s="43" t="n">
         <v>0.875</v>
       </c>
       <c r="K69" s="16" t="s">
@@ -6654,7 +6642,7 @@
       <c r="B70" s="15" t="n">
         <v>26</v>
       </c>
-      <c r="C70" s="36" t="s">
+      <c r="C70" s="34" t="s">
         <v>311</v>
       </c>
       <c r="D70" s="10" t="s">
@@ -6675,7 +6663,7 @@
       <c r="I70" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="J70" s="44" t="n">
+      <c r="J70" s="42" t="n">
         <v>0.875</v>
       </c>
       <c r="K70" s="10" t="s">
@@ -6710,7 +6698,7 @@
       <c r="I71" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="J71" s="44" t="n">
+      <c r="J71" s="42" t="n">
         <v>0.875</v>
       </c>
       <c r="K71" s="10" t="s">
@@ -6745,7 +6733,7 @@
       <c r="I72" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="J72" s="46" t="n">
+      <c r="J72" s="44" t="n">
         <v>0.875</v>
       </c>
       <c r="K72" s="18" t="s">
@@ -6780,7 +6768,7 @@
       <c r="I73" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="J73" s="45" t="n">
+      <c r="J73" s="43" t="n">
         <v>0.875</v>
       </c>
       <c r="K73" s="16" t="s">
@@ -6829,7 +6817,7 @@
       <c r="B75" s="8" t="n">
         <v>204</v>
       </c>
-      <c r="C75" s="36" t="s">
+      <c r="C75" s="34" t="s">
         <v>330</v>
       </c>
       <c r="D75" s="7" t="s">
@@ -6850,7 +6838,7 @@
       <c r="I75" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="J75" s="43" t="n">
+      <c r="J75" s="41" t="n">
         <v>2.25</v>
       </c>
       <c r="K75" s="10" t="s">
@@ -6900,7 +6888,7 @@
       <c r="I77" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="J77" s="44" t="n">
+      <c r="J77" s="42" t="n">
         <v>0.875</v>
       </c>
       <c r="K77" s="10" t="s">
@@ -6985,7 +6973,7 @@
       <c r="I80" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="J80" s="44" t="n">
+      <c r="J80" s="42" t="n">
         <v>0.625</v>
       </c>
       <c r="K80" s="10" t="s">
@@ -6996,7 +6984,7 @@
       <c r="A81" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="B81" s="27" t="s">
+      <c r="B81" s="26" t="s">
         <v>37</v>
       </c>
       <c r="C81" s="7" t="s">
@@ -7055,7 +7043,7 @@
       <c r="I82" s="10" t="s">
         <v>355</v>
       </c>
-      <c r="J82" s="44" t="n">
+      <c r="J82" s="42" t="n">
         <v>0.625</v>
       </c>
       <c r="K82" s="10" t="s">
@@ -7069,7 +7057,7 @@
       <c r="B83" s="20" t="n">
         <v>78</v>
       </c>
-      <c r="C83" s="41" t="s">
+      <c r="C83" s="39" t="s">
         <v>357</v>
       </c>
       <c r="D83" s="16" t="s">
@@ -7090,7 +7078,7 @@
       <c r="I83" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="J83" s="45" t="n">
+      <c r="J83" s="43" t="n">
         <v>0.625</v>
       </c>
       <c r="K83" s="16" t="s">
@@ -7104,7 +7092,7 @@
       <c r="B84" s="20" t="n">
         <v>80</v>
       </c>
-      <c r="C84" s="42" t="s">
+      <c r="C84" s="40" t="s">
         <v>361</v>
       </c>
       <c r="D84" s="16" t="s">
@@ -7125,7 +7113,7 @@
       <c r="I84" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="J84" s="45" t="n">
+      <c r="J84" s="43" t="n">
         <v>0.625</v>
       </c>
       <c r="K84" s="16" t="s">
@@ -7160,7 +7148,7 @@
       <c r="I85" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="J85" s="46" t="n">
+      <c r="J85" s="44" t="n">
         <v>0.625</v>
       </c>
       <c r="K85" s="18" t="s">
@@ -7195,7 +7183,7 @@
       <c r="I86" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="J86" s="44" t="n">
+      <c r="J86" s="42" t="n">
         <v>0.625</v>
       </c>
       <c r="K86" s="10" t="s">
@@ -7345,7 +7333,7 @@
       <c r="I92" s="10" t="s">
         <v>383</v>
       </c>
-      <c r="J92" s="28" t="n">
+      <c r="J92" s="27" t="n">
         <v>4</v>
       </c>
       <c r="K92" s="10" t="s">
@@ -7374,7 +7362,7 @@
       <c r="B94" s="8" t="n">
         <v>32</v>
       </c>
-      <c r="C94" s="27" t="s">
+      <c r="C94" s="26" t="s">
         <v>100</v>
       </c>
       <c r="D94" s="7" t="s">
@@ -7389,7 +7377,7 @@
       <c r="G94" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="H94" s="30" t="s">
+      <c r="H94" s="10" t="s">
         <v>389</v>
       </c>
       <c r="I94" s="7" t="s">
@@ -7444,7 +7432,7 @@
       <c r="B96" s="8" t="n">
         <v>206</v>
       </c>
-      <c r="C96" s="27" t="s">
+      <c r="C96" s="26" t="s">
         <v>77</v>
       </c>
       <c r="D96" s="7" t="s">
@@ -7459,10 +7447,10 @@
       <c r="G96" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="H96" s="30" t="s">
+      <c r="H96" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="I96" s="30" t="s">
+      <c r="I96" s="10" t="s">
         <v>398</v>
       </c>
       <c r="J96" s="11" t="n">
@@ -7515,7 +7503,7 @@
       <c r="I98" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="J98" s="28" t="n">
+      <c r="J98" s="27" t="n">
         <v>2</v>
       </c>
       <c r="K98" s="10" t="s">
@@ -7547,7 +7535,7 @@
       <c r="H99" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="I99" s="30" t="s">
+      <c r="I99" s="10" t="s">
         <v>410</v>
       </c>
       <c r="J99" s="11" t="n">
@@ -7564,7 +7552,7 @@
       <c r="B100" s="15" t="n">
         <v>36</v>
       </c>
-      <c r="C100" s="38" t="s">
+      <c r="C100" s="36" t="s">
         <v>413</v>
       </c>
       <c r="D100" s="10" t="s">
@@ -7585,7 +7573,7 @@
       <c r="I100" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="J100" s="28" t="n">
+      <c r="J100" s="27" t="n">
         <v>2</v>
       </c>
       <c r="K100" s="10" t="s">
@@ -7649,13 +7637,13 @@
       <c r="G102" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="H102" s="25" t="s">
+      <c r="H102" s="16" t="s">
         <v>421</v>
       </c>
       <c r="I102" s="18" t="s">
         <v>422</v>
       </c>
-      <c r="J102" s="35" t="n">
+      <c r="J102" s="33" t="n">
         <v>2</v>
       </c>
       <c r="K102" s="18" t="s">
@@ -7669,7 +7657,7 @@
       <c r="B103" s="24" t="n">
         <v>60</v>
       </c>
-      <c r="C103" s="41" t="s">
+      <c r="C103" s="39" t="s">
         <v>424</v>
       </c>
       <c r="D103" s="18" t="s">
@@ -7684,13 +7672,13 @@
       <c r="G103" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="H103" s="25" t="s">
+      <c r="H103" s="16" t="s">
         <v>425</v>
       </c>
-      <c r="I103" s="25" t="s">
+      <c r="I103" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="J103" s="35" t="n">
+      <c r="J103" s="33" t="n">
         <v>2</v>
       </c>
       <c r="K103" s="16" t="s">
@@ -7704,7 +7692,7 @@
       <c r="B104" s="8" t="n">
         <v>59</v>
       </c>
-      <c r="C104" s="36" t="s">
+      <c r="C104" s="34" t="s">
         <v>429</v>
       </c>
       <c r="D104" s="7" t="s">
@@ -7754,13 +7742,13 @@
       <c r="G105" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="H105" s="30" t="s">
+      <c r="H105" s="10" t="s">
         <v>436</v>
       </c>
       <c r="I105" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="J105" s="43" t="n">
+      <c r="J105" s="41" t="n">
         <v>2</v>
       </c>
       <c r="K105" s="7" t="s">
@@ -7774,7 +7762,7 @@
       <c r="B106" s="15" t="n">
         <v>58</v>
       </c>
-      <c r="C106" s="36" t="s">
+      <c r="C106" s="34" t="s">
         <v>439</v>
       </c>
       <c r="D106" s="10" t="s">
@@ -7795,7 +7783,7 @@
       <c r="I106" s="10" t="s">
         <v>440</v>
       </c>
-      <c r="J106" s="28" t="n">
+      <c r="J106" s="27" t="n">
         <v>2</v>
       </c>
       <c r="K106" s="10" t="s">
@@ -7880,7 +7868,7 @@
       <c r="I109" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="J109" s="28" t="n">
+      <c r="J109" s="27" t="n">
         <v>1.5</v>
       </c>
       <c r="K109" s="10" t="s">
@@ -7909,7 +7897,7 @@
       <c r="B111" s="8" t="n">
         <v>61</v>
       </c>
-      <c r="C111" s="27" t="s">
+      <c r="C111" s="26" t="s">
         <v>401</v>
       </c>
       <c r="D111" s="7" t="s">
@@ -7924,13 +7912,13 @@
       <c r="G111" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="H111" s="30" t="s">
+      <c r="H111" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="I111" s="30" t="s">
+      <c r="I111" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="J111" s="43" t="n">
+      <c r="J111" s="41" t="n">
         <v>1.25</v>
       </c>
       <c r="K111" s="10" t="s">
@@ -7944,7 +7932,7 @@
       <c r="B112" s="24" t="n">
         <v>104</v>
       </c>
-      <c r="C112" s="39" t="s">
+      <c r="C112" s="37" t="s">
         <v>456</v>
       </c>
       <c r="D112" s="18" t="s">
@@ -7959,13 +7947,13 @@
       <c r="G112" s="18" t="s">
         <v>451</v>
       </c>
-      <c r="H112" s="25" t="s">
+      <c r="H112" s="16" t="s">
         <v>457</v>
       </c>
-      <c r="I112" s="25" t="s">
+      <c r="I112" s="16" t="s">
         <v>458</v>
       </c>
-      <c r="J112" s="26" t="n">
+      <c r="J112" s="25" t="n">
         <v>1.25</v>
       </c>
       <c r="K112" s="18" t="s">
@@ -7979,7 +7967,7 @@
       <c r="B113" s="24" t="n">
         <v>131</v>
       </c>
-      <c r="C113" s="39" t="s">
+      <c r="C113" s="37" t="s">
         <v>429</v>
       </c>
       <c r="D113" s="18" t="s">
@@ -7994,13 +7982,13 @@
       <c r="G113" s="18" t="s">
         <v>451</v>
       </c>
-      <c r="H113" s="25" t="s">
+      <c r="H113" s="16" t="s">
         <v>461</v>
       </c>
-      <c r="I113" s="25" t="s">
+      <c r="I113" s="16" t="s">
         <v>462</v>
       </c>
-      <c r="J113" s="26" t="n">
+      <c r="J113" s="25" t="n">
         <v>1.25</v>
       </c>
       <c r="K113" s="18" t="s">
@@ -8029,13 +8017,13 @@
       <c r="G114" s="7" t="s">
         <v>451</v>
       </c>
-      <c r="H114" s="30" t="s">
+      <c r="H114" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="I114" s="30" t="s">
+      <c r="I114" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="J114" s="43" t="n">
+      <c r="J114" s="41" t="n">
         <v>1.25</v>
       </c>
       <c r="K114" s="7" t="s">
@@ -8099,7 +8087,7 @@
       <c r="B117" s="8" t="n">
         <v>63</v>
       </c>
-      <c r="C117" s="27" t="s">
+      <c r="C117" s="26" t="s">
         <v>476</v>
       </c>
       <c r="D117" s="7" t="s">
@@ -8114,7 +8102,7 @@
       <c r="G117" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="H117" s="30" t="s">
+      <c r="H117" s="10" t="s">
         <v>478</v>
       </c>
       <c r="I117" s="7" t="s">
@@ -8134,7 +8122,7 @@
       <c r="B118" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="C118" s="41" t="s">
+      <c r="C118" s="39" t="s">
         <v>482</v>
       </c>
       <c r="D118" s="16" t="s">
@@ -8169,7 +8157,7 @@
       <c r="B119" s="20" t="n">
         <v>55</v>
       </c>
-      <c r="C119" s="42" t="s">
+      <c r="C119" s="40" t="s">
         <v>306</v>
       </c>
       <c r="D119" s="16" t="s">
@@ -8204,7 +8192,7 @@
       <c r="B120" s="8" t="n">
         <v>207</v>
       </c>
-      <c r="C120" s="27" t="s">
+      <c r="C120" s="26" t="s">
         <v>147</v>
       </c>
       <c r="D120" s="7" t="s">
@@ -8219,13 +8207,13 @@
       <c r="G120" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="H120" s="30" t="s">
+      <c r="H120" s="10" t="s">
         <v>488</v>
       </c>
       <c r="I120" s="7" t="s">
         <v>489</v>
       </c>
-      <c r="J120" s="43" t="n">
+      <c r="J120" s="41" t="n">
         <v>2.25</v>
       </c>
       <c r="K120" s="7" t="s">
@@ -8239,7 +8227,7 @@
       <c r="B121" s="8" t="n">
         <v>208</v>
       </c>
-      <c r="C121" s="37" t="s">
+      <c r="C121" s="35" t="s">
         <v>330</v>
       </c>
       <c r="D121" s="7" t="s">
@@ -8254,16 +8242,16 @@
       <c r="G121" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="H121" s="30" t="s">
+      <c r="H121" s="10" t="s">
         <v>491</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="J121" s="43" t="n">
+      <c r="J121" s="41" t="n">
         <v>2.25</v>
       </c>
-      <c r="K121" s="30" t="s">
+      <c r="K121" s="10" t="s">
         <v>493</v>
       </c>
     </row>
@@ -8310,7 +8298,7 @@
       <c r="I123" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="J123" s="44" t="n">
+      <c r="J123" s="42" t="n">
         <v>0.625</v>
       </c>
       <c r="K123" s="10" t="s">
@@ -8324,7 +8312,7 @@
       <c r="B124" s="20" t="n">
         <v>67</v>
       </c>
-      <c r="C124" s="42" t="s">
+      <c r="C124" s="40" t="s">
         <v>361</v>
       </c>
       <c r="D124" s="16" t="s">
@@ -8345,7 +8333,7 @@
       <c r="I124" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="J124" s="45" t="n">
+      <c r="J124" s="43" t="n">
         <v>0.625</v>
       </c>
       <c r="K124" s="16" t="s">
@@ -8359,7 +8347,7 @@
       <c r="B125" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="C125" s="36" t="s">
+      <c r="C125" s="34" t="s">
         <v>505</v>
       </c>
       <c r="D125" s="7" t="s">
@@ -8380,7 +8368,7 @@
       <c r="I125" s="7" t="s">
         <v>508</v>
       </c>
-      <c r="J125" s="43" t="n">
+      <c r="J125" s="41" t="n">
         <v>0.63</v>
       </c>
       <c r="K125" s="10" t="s">
@@ -8445,7 +8433,7 @@
       <c r="I128" s="10" t="s">
         <v>514</v>
       </c>
-      <c r="J128" s="28" t="n">
+      <c r="J128" s="27" t="n">
         <v>3</v>
       </c>
       <c r="K128" s="10" t="s">
@@ -8509,7 +8497,7 @@
       <c r="B131" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="C131" s="27" t="s">
+      <c r="C131" s="26" t="s">
         <v>476</v>
       </c>
       <c r="D131" s="7" t="s">
@@ -8527,7 +8515,7 @@
       <c r="H131" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I131" s="30" t="s">
+      <c r="I131" s="10" t="s">
         <v>524</v>
       </c>
       <c r="J131" s="11" t="n">
@@ -8544,7 +8532,7 @@
       <c r="B132" s="8" t="n">
         <v>53</v>
       </c>
-      <c r="C132" s="36" t="s">
+      <c r="C132" s="34" t="s">
         <v>526</v>
       </c>
       <c r="D132" s="7" t="s">
@@ -8559,7 +8547,7 @@
       <c r="G132" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="H132" s="30" t="s">
+      <c r="H132" s="10" t="s">
         <v>527</v>
       </c>
       <c r="I132" s="7" t="s">
@@ -8635,7 +8623,7 @@
       <c r="I134" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J134" s="28" t="n">
+      <c r="J134" s="27" t="n">
         <v>4.5</v>
       </c>
       <c r="K134" s="10" t="s">
@@ -8670,7 +8658,7 @@
       <c r="I135" s="16" t="s">
         <v>537</v>
       </c>
-      <c r="J135" s="29" t="n">
+      <c r="J135" s="28" t="n">
         <v>1.5</v>
       </c>
       <c r="K135" s="16" t="s">
@@ -8684,7 +8672,7 @@
       <c r="B136" s="20" t="n">
         <v>12</v>
       </c>
-      <c r="C136" s="41" t="s">
+      <c r="C136" s="39" t="s">
         <v>540</v>
       </c>
       <c r="D136" s="16" t="s">
@@ -8705,7 +8693,7 @@
       <c r="I136" s="16" t="s">
         <v>542</v>
       </c>
-      <c r="J136" s="29" t="n">
+      <c r="J136" s="28" t="n">
         <v>1.5</v>
       </c>
       <c r="K136" s="16" t="s">
@@ -8754,7 +8742,7 @@
       <c r="B138" s="15" t="n">
         <v>106</v>
       </c>
-      <c r="C138" s="36" t="s">
+      <c r="C138" s="34" t="s">
         <v>549</v>
       </c>
       <c r="D138" s="10" t="s">
@@ -8775,7 +8763,7 @@
       <c r="I138" s="10" t="s">
         <v>551</v>
       </c>
-      <c r="J138" s="28" t="n">
+      <c r="J138" s="27" t="n">
         <v>1.5</v>
       </c>
       <c r="K138" s="10" t="s">
@@ -8810,7 +8798,7 @@
       <c r="I139" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="J139" s="28" t="n">
+      <c r="J139" s="27" t="n">
         <v>2.5</v>
       </c>
       <c r="K139" s="10" t="s">
@@ -8839,7 +8827,7 @@
       <c r="B141" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="C141" s="38" t="s">
+      <c r="C141" s="36" t="s">
         <v>557</v>
       </c>
       <c r="D141" s="10" t="s">
@@ -8860,7 +8848,7 @@
       <c r="I141" s="10" t="s">
         <v>560</v>
       </c>
-      <c r="J141" s="28" t="n">
+      <c r="J141" s="27" t="n">
         <v>1.5</v>
       </c>
       <c r="K141" s="10" t="s">
@@ -8924,7 +8912,7 @@
       <c r="B144" s="15" t="n">
         <v>69</v>
       </c>
-      <c r="C144" s="38" t="s">
+      <c r="C144" s="36" t="s">
         <v>306</v>
       </c>
       <c r="D144" s="10" t="s">
@@ -8959,7 +8947,7 @@
       <c r="B145" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C145" s="47" t="s">
+      <c r="C145" s="21" t="s">
         <v>571</v>
       </c>
       <c r="D145" s="18" t="s">
@@ -8994,7 +8982,7 @@
       <c r="B146" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C146" s="47" t="s">
+      <c r="C146" s="21" t="s">
         <v>573</v>
       </c>
       <c r="D146" s="17" t="s">
@@ -9064,7 +9052,7 @@
       <c r="B148" s="15" t="n">
         <v>88</v>
       </c>
-      <c r="C148" s="36" t="s">
+      <c r="C148" s="34" t="s">
         <v>581</v>
       </c>
       <c r="D148" s="10" t="s">
@@ -9120,7 +9108,7 @@
       <c r="I149" s="7" t="s">
         <v>588</v>
       </c>
-      <c r="J149" s="43" t="n">
+      <c r="J149" s="41" t="n">
         <v>2.25</v>
       </c>
       <c r="K149" s="10" t="s">
@@ -9170,7 +9158,7 @@
       <c r="I151" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="J151" s="44" t="n">
+      <c r="J151" s="42" t="n">
         <v>0.625</v>
       </c>
       <c r="K151" s="10" t="s">
@@ -9240,7 +9228,7 @@
       <c r="I153" s="18" t="s">
         <v>603</v>
       </c>
-      <c r="J153" s="35" t="n">
+      <c r="J153" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K153" s="18" t="s">
@@ -9254,7 +9242,7 @@
       <c r="B154" s="8" t="n">
         <v>68</v>
       </c>
-      <c r="C154" s="38" t="s">
+      <c r="C154" s="36" t="s">
         <v>361</v>
       </c>
       <c r="D154" s="7" t="s">
@@ -9269,13 +9257,13 @@
       <c r="G154" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="H154" s="30" t="s">
+      <c r="H154" s="10" t="s">
         <v>606</v>
       </c>
       <c r="I154" s="7" t="s">
         <v>607</v>
       </c>
-      <c r="J154" s="48" t="n">
+      <c r="J154" s="45" t="n">
         <v>0.625</v>
       </c>
       <c r="K154" s="7" t="s">
@@ -9337,7 +9325,7 @@
       <c r="H157" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I157" s="30" t="s">
+      <c r="I157" s="10" t="s">
         <v>613</v>
       </c>
       <c r="J157" s="11" t="n">
@@ -9354,7 +9342,7 @@
       <c r="B158" s="8" t="n">
         <v>120</v>
       </c>
-      <c r="C158" s="36" t="s">
+      <c r="C158" s="34" t="s">
         <v>616</v>
       </c>
       <c r="D158" s="7" t="s">
@@ -9425,7 +9413,7 @@
       <c r="I160" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="J160" s="28" t="n">
+      <c r="J160" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K160" s="10" t="s">
@@ -9460,7 +9448,7 @@
       <c r="I161" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="J161" s="28" t="n">
+      <c r="J161" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K161" s="10" t="s">
@@ -9510,7 +9498,7 @@
       <c r="I163" s="10" t="s">
         <v>634</v>
       </c>
-      <c r="J163" s="28" t="n">
+      <c r="J163" s="27" t="n">
         <v>2</v>
       </c>
       <c r="K163" s="10" t="s">
@@ -9580,7 +9568,7 @@
       <c r="I165" s="18" t="s">
         <v>640</v>
       </c>
-      <c r="J165" s="35" t="n">
+      <c r="J165" s="33" t="n">
         <v>0.5</v>
       </c>
       <c r="K165" s="18" t="s">
@@ -9615,7 +9603,7 @@
       <c r="I166" s="18" t="s">
         <v>646</v>
       </c>
-      <c r="J166" s="26" t="n">
+      <c r="J166" s="25" t="n">
         <v>0.75</v>
       </c>
       <c r="K166" s="18" t="s">
@@ -9676,16 +9664,16 @@
       <c r="A169" s="10" t="s">
         <v>652</v>
       </c>
-      <c r="B169" s="30"/>
-      <c r="C169" s="30"/>
-      <c r="D169" s="30"/>
-      <c r="E169" s="30"/>
-      <c r="F169" s="30"/>
-      <c r="G169" s="30"/>
-      <c r="H169" s="30"/>
-      <c r="I169" s="30"/>
-      <c r="J169" s="30"/>
-      <c r="K169" s="30"/>
+      <c r="B169" s="10"/>
+      <c r="C169" s="10"/>
+      <c r="D169" s="10"/>
+      <c r="E169" s="10"/>
+      <c r="F169" s="10"/>
+      <c r="G169" s="10"/>
+      <c r="H169" s="10"/>
+      <c r="I169" s="10"/>
+      <c r="J169" s="10"/>
+      <c r="K169" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="170">
       <c r="A170" s="5" t="s">
@@ -9730,7 +9718,7 @@
       <c r="I171" s="10" t="s">
         <v>658</v>
       </c>
-      <c r="J171" s="28" t="n">
+      <c r="J171" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K171" s="10" t="s">
@@ -9765,7 +9753,7 @@
       <c r="I172" s="10" t="s">
         <v>662</v>
       </c>
-      <c r="J172" s="28" t="n">
+      <c r="J172" s="27" t="n">
         <v>1</v>
       </c>
       <c r="K172" s="10" t="s">
@@ -9800,7 +9788,7 @@
       <c r="I173" s="10" t="s">
         <v>666</v>
       </c>
-      <c r="J173" s="28" t="n">
+      <c r="J173" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K173" s="10" t="s">
@@ -9814,7 +9802,7 @@
       <c r="B174" s="18" t="s">
         <v>669</v>
       </c>
-      <c r="C174" s="41" t="s">
+      <c r="C174" s="39" t="s">
         <v>670</v>
       </c>
       <c r="D174" s="18" t="s">
@@ -9835,7 +9823,7 @@
       <c r="I174" s="18" t="s">
         <v>672</v>
       </c>
-      <c r="J174" s="35" t="n">
+      <c r="J174" s="33" t="n">
         <v>1</v>
       </c>
       <c r="K174" s="16" t="s">
@@ -9870,7 +9858,7 @@
       <c r="I175" s="16" t="s">
         <v>677</v>
       </c>
-      <c r="J175" s="29" t="n">
+      <c r="J175" s="28" t="n">
         <v>1</v>
       </c>
       <c r="K175" s="16" t="s">
@@ -9905,7 +9893,7 @@
       <c r="I176" s="18" t="s">
         <v>683</v>
       </c>
-      <c r="J176" s="35" t="n">
+      <c r="J176" s="33" t="n">
         <v>1</v>
       </c>
       <c r="K176" s="16" t="s">
@@ -9919,7 +9907,7 @@
       <c r="B177" s="8" t="n">
         <v>31</v>
       </c>
-      <c r="C177" s="37" t="s">
+      <c r="C177" s="35" t="s">
         <v>686</v>
       </c>
       <c r="D177" s="7" t="s">
@@ -9934,7 +9922,7 @@
       <c r="G177" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="H177" s="30" t="s">
+      <c r="H177" s="10" t="s">
         <v>687</v>
       </c>
       <c r="I177" s="7" t="s">
@@ -9954,7 +9942,7 @@
       <c r="B178" s="7" t="s">
         <v>691</v>
       </c>
-      <c r="C178" s="36" t="s">
+      <c r="C178" s="34" t="s">
         <v>692</v>
       </c>
       <c r="D178" s="7" t="s">
@@ -10025,7 +10013,7 @@
       <c r="I180" s="10" t="s">
         <v>699</v>
       </c>
-      <c r="J180" s="28" t="n">
+      <c r="J180" s="27" t="n">
         <v>0.5</v>
       </c>
       <c r="K180" s="10" t="s">
@@ -10039,7 +10027,7 @@
       <c r="B181" s="7" t="s">
         <v>702</v>
       </c>
-      <c r="C181" s="36" t="s">
+      <c r="C181" s="34" t="s">
         <v>703</v>
       </c>
       <c r="D181" s="7" t="s">
@@ -10095,7 +10083,7 @@
       <c r="I182" s="16" t="s">
         <v>709</v>
       </c>
-      <c r="J182" s="29" t="n">
+      <c r="J182" s="28" t="n">
         <v>0.5</v>
       </c>
       <c r="K182" s="16" t="s">
@@ -10144,7 +10132,7 @@
       <c r="B184" s="7" t="s">
         <v>718</v>
       </c>
-      <c r="C184" s="36" t="s">
+      <c r="C184" s="34" t="s">
         <v>719</v>
       </c>
       <c r="D184" s="7" t="s">
@@ -10215,7 +10203,7 @@
       <c r="I186" s="10" t="s">
         <v>728</v>
       </c>
-      <c r="J186" s="28" t="n">
+      <c r="J186" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K186" s="10" t="s">
@@ -10247,7 +10235,7 @@
       <c r="H187" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I187" s="30" t="s">
+      <c r="I187" s="10" t="s">
         <v>733</v>
       </c>
       <c r="J187" s="11" t="n">
@@ -10279,7 +10267,7 @@
       <c r="G188" s="7" t="s">
         <v>737</v>
       </c>
-      <c r="H188" s="27" t="s">
+      <c r="H188" s="26" t="s">
         <v>72</v>
       </c>
       <c r="I188" s="7" t="s">
@@ -10320,10 +10308,10 @@
       <c r="I189" s="18" t="s">
         <v>744</v>
       </c>
-      <c r="J189" s="35" t="n">
+      <c r="J189" s="33" t="n">
         <v>0</v>
       </c>
-      <c r="K189" s="25" t="s">
+      <c r="K189" s="16" t="s">
         <v>745</v>
       </c>
     </row>
@@ -10384,13 +10372,13 @@
       <c r="G191" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H191" s="25" t="s">
+      <c r="H191" s="16" t="s">
         <v>749</v>
       </c>
       <c r="I191" s="18" t="s">
         <v>750</v>
       </c>
-      <c r="J191" s="35" t="n">
+      <c r="J191" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K191" s="18" t="s">
@@ -10439,7 +10427,7 @@
       <c r="B193" s="8" t="n">
         <v>45</v>
       </c>
-      <c r="C193" s="38" t="s">
+      <c r="C193" s="36" t="s">
         <v>757</v>
       </c>
       <c r="D193" s="7" t="s">
@@ -10545,7 +10533,7 @@
       <c r="I196" s="10" t="s">
         <v>770</v>
       </c>
-      <c r="J196" s="28" t="n">
+      <c r="J196" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K196" s="10" t="s">
@@ -10580,7 +10568,7 @@
       <c r="I197" s="18" t="s">
         <v>775</v>
       </c>
-      <c r="J197" s="35" t="n">
+      <c r="J197" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K197" s="16" t="s">
@@ -10644,7 +10632,7 @@
       <c r="B200" s="10" t="s">
         <v>785</v>
       </c>
-      <c r="C200" s="36" t="s">
+      <c r="C200" s="34" t="s">
         <v>786</v>
       </c>
       <c r="D200" s="10" t="s">
@@ -10665,7 +10653,7 @@
       <c r="I200" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J200" s="28" t="n">
+      <c r="J200" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K200" s="10" t="s">
@@ -10679,7 +10667,7 @@
       <c r="B201" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="C201" s="37" t="s">
+      <c r="C201" s="35" t="s">
         <v>791</v>
       </c>
       <c r="D201" s="7" t="s">
@@ -10694,7 +10682,7 @@
       <c r="G201" s="7" t="s">
         <v>792</v>
       </c>
-      <c r="H201" s="30" t="s">
+      <c r="H201" s="10" t="s">
         <v>793</v>
       </c>
       <c r="I201" s="7" t="s">
@@ -10714,7 +10702,7 @@
       <c r="B202" s="15" t="n">
         <v>24</v>
       </c>
-      <c r="C202" s="38" t="s">
+      <c r="C202" s="36" t="s">
         <v>796</v>
       </c>
       <c r="D202" s="10" t="s">
@@ -10735,7 +10723,7 @@
       <c r="I202" s="10" t="s">
         <v>770</v>
       </c>
-      <c r="J202" s="28" t="n">
+      <c r="J202" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K202" s="10" t="s">
@@ -10749,7 +10737,7 @@
       <c r="B203" s="15" t="n">
         <v>24</v>
       </c>
-      <c r="C203" s="38" t="s">
+      <c r="C203" s="36" t="s">
         <v>800</v>
       </c>
       <c r="D203" s="10" t="s">
@@ -10770,7 +10758,7 @@
       <c r="I203" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="J203" s="28" t="n">
+      <c r="J203" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K203" s="10" t="s">
@@ -10784,7 +10772,7 @@
       <c r="B204" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="C204" s="41" t="s">
+      <c r="C204" s="39" t="s">
         <v>803</v>
       </c>
       <c r="D204" s="16" t="s">
@@ -10805,7 +10793,7 @@
       <c r="I204" s="16" t="s">
         <v>804</v>
       </c>
-      <c r="J204" s="29" t="n">
+      <c r="J204" s="28" t="n">
         <v>0</v>
       </c>
       <c r="K204" s="16" t="s">
@@ -10840,7 +10828,7 @@
       <c r="I205" s="16" t="s">
         <v>808</v>
       </c>
-      <c r="J205" s="29" t="n">
+      <c r="J205" s="28" t="n">
         <v>0</v>
       </c>
       <c r="K205" s="16" t="s">
@@ -10854,7 +10842,7 @@
       <c r="B206" s="7" t="s">
         <v>811</v>
       </c>
-      <c r="C206" s="36" t="s">
+      <c r="C206" s="34" t="s">
         <v>812</v>
       </c>
       <c r="D206" s="7" t="s">
@@ -10883,13 +10871,13 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="21" outlineLevel="0" r="207">
-      <c r="A207" s="30" t="s">
+      <c r="A207" s="10" t="s">
         <v>817</v>
       </c>
       <c r="B207" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="C207" s="27" t="s">
+      <c r="C207" s="26" t="s">
         <v>818</v>
       </c>
       <c r="D207" s="7" t="s">
@@ -10924,7 +10912,7 @@
       <c r="B208" s="8" t="n">
         <v>202</v>
       </c>
-      <c r="C208" s="37" t="s">
+      <c r="C208" s="35" t="s">
         <v>822</v>
       </c>
       <c r="D208" s="7" t="s">
@@ -10939,7 +10927,7 @@
       <c r="G208" s="7" t="s">
         <v>823</v>
       </c>
-      <c r="H208" s="30" t="s">
+      <c r="H208" s="10" t="s">
         <v>824</v>
       </c>
       <c r="I208" s="7" t="s">
@@ -10959,7 +10947,7 @@
       <c r="B209" s="18" t="s">
         <v>827</v>
       </c>
-      <c r="C209" s="41" t="s">
+      <c r="C209" s="39" t="s">
         <v>828</v>
       </c>
       <c r="D209" s="18" t="s">
@@ -10974,13 +10962,13 @@
       <c r="G209" s="18" t="s">
         <v>787</v>
       </c>
-      <c r="H209" s="25" t="s">
+      <c r="H209" s="16" t="s">
         <v>829</v>
       </c>
       <c r="I209" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J209" s="35" t="n">
+      <c r="J209" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K209" s="18" t="s">
@@ -10994,7 +10982,7 @@
       <c r="B210" s="16" t="s">
         <v>831</v>
       </c>
-      <c r="C210" s="42" t="s">
+      <c r="C210" s="40" t="s">
         <v>832</v>
       </c>
       <c r="D210" s="18" t="s">
@@ -11009,13 +10997,13 @@
       <c r="G210" s="18" t="s">
         <v>833</v>
       </c>
-      <c r="H210" s="25" t="s">
+      <c r="H210" s="16" t="s">
         <v>834</v>
       </c>
       <c r="I210" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J210" s="35" t="n">
+      <c r="J210" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K210" s="18" t="s">
@@ -11050,7 +11038,7 @@
       <c r="I211" s="10" t="s">
         <v>838</v>
       </c>
-      <c r="J211" s="28" t="n">
+      <c r="J211" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K211" s="10" t="s">
@@ -11064,7 +11052,7 @@
       <c r="B212" s="10" t="s">
         <v>841</v>
       </c>
-      <c r="C212" s="36" t="s">
+      <c r="C212" s="34" t="s">
         <v>842</v>
       </c>
       <c r="D212" s="7" t="s">
@@ -11079,7 +11067,7 @@
       <c r="G212" s="7" t="s">
         <v>813</v>
       </c>
-      <c r="H212" s="30" t="s">
+      <c r="H212" s="10" t="s">
         <v>843</v>
       </c>
       <c r="I212" s="7" t="s">
@@ -11167,7 +11155,7 @@
       <c r="H215" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I215" s="30" t="s">
+      <c r="I215" s="10" t="s">
         <v>848</v>
       </c>
       <c r="J215" s="11" t="n">
@@ -11202,7 +11190,7 @@
       <c r="H216" s="7" t="s">
         <v>852</v>
       </c>
-      <c r="I216" s="30" t="s">
+      <c r="I216" s="10" t="s">
         <v>853</v>
       </c>
       <c r="J216" s="11" t="n">
@@ -11240,7 +11228,7 @@
       <c r="I217" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J217" s="35" t="n">
+      <c r="J217" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K217" s="16" t="s">
@@ -11275,7 +11263,7 @@
       <c r="I218" s="16" t="s">
         <v>860</v>
       </c>
-      <c r="J218" s="29" t="n">
+      <c r="J218" s="28" t="n">
         <v>0</v>
       </c>
       <c r="K218" s="16" t="s">
@@ -11430,7 +11418,7 @@
       <c r="I223" s="10" t="s">
         <v>666</v>
       </c>
-      <c r="J223" s="28" t="n">
+      <c r="J223" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K223" s="10" t="s">
@@ -11444,7 +11432,7 @@
       <c r="B224" s="7" t="s">
         <v>731</v>
       </c>
-      <c r="C224" s="27" t="s">
+      <c r="C224" s="26" t="s">
         <v>876</v>
       </c>
       <c r="D224" s="7" t="s">
@@ -11456,7 +11444,7 @@
       <c r="F224" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="G224" s="27" t="s">
+      <c r="G224" s="26" t="s">
         <v>731</v>
       </c>
       <c r="H224" s="7" t="s">
@@ -11473,13 +11461,13 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="225">
-      <c r="A225" s="41" t="s">
+      <c r="A225" s="39" t="s">
         <v>879</v>
       </c>
       <c r="B225" s="16" t="s">
         <v>731</v>
       </c>
-      <c r="C225" s="41" t="s">
+      <c r="C225" s="39" t="s">
         <v>879</v>
       </c>
       <c r="D225" s="16" t="s">
@@ -11500,7 +11488,7 @@
       <c r="I225" s="16" t="s">
         <v>880</v>
       </c>
-      <c r="J225" s="29" t="n">
+      <c r="J225" s="28" t="n">
         <v>0</v>
       </c>
       <c r="K225" s="16" t="s">
@@ -11523,7 +11511,7 @@
       <c r="E226" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="F226" s="25" t="s">
+      <c r="F226" s="16" t="s">
         <v>884</v>
       </c>
       <c r="G226" s="18" t="s">
@@ -11535,7 +11523,7 @@
       <c r="I226" s="18" t="s">
         <v>885</v>
       </c>
-      <c r="J226" s="35" t="n">
+      <c r="J226" s="33" t="n">
         <v>0</v>
       </c>
       <c r="K226" s="18" t="s">
@@ -11549,7 +11537,7 @@
       <c r="B227" s="7" t="s">
         <v>888</v>
       </c>
-      <c r="C227" s="27" t="s">
+      <c r="C227" s="26" t="s">
         <v>37</v>
       </c>
       <c r="D227" s="7" t="s">
@@ -11605,7 +11593,7 @@
       <c r="I228" s="10" t="s">
         <v>895</v>
       </c>
-      <c r="J228" s="28" t="n">
+      <c r="J228" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K228" s="10" t="s">
@@ -11640,7 +11628,7 @@
       <c r="I229" s="10" t="s">
         <v>900</v>
       </c>
-      <c r="J229" s="28" t="n">
+      <c r="J229" s="27" t="n">
         <v>0</v>
       </c>
       <c r="K229" s="10" t="s">
@@ -11648,19 +11636,19 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12" outlineLevel="0" r="230">
-      <c r="A230" s="49" t="s">
+      <c r="A230" s="46" t="s">
         <v>902</v>
       </c>
-      <c r="B230" s="49"/>
-      <c r="C230" s="49"/>
-      <c r="D230" s="49"/>
-      <c r="E230" s="49"/>
-      <c r="F230" s="49"/>
-      <c r="G230" s="49"/>
-      <c r="H230" s="49"/>
-      <c r="I230" s="49"/>
-      <c r="J230" s="49"/>
-      <c r="K230" s="49"/>
+      <c r="B230" s="46"/>
+      <c r="C230" s="46"/>
+      <c r="D230" s="46"/>
+      <c r="E230" s="46"/>
+      <c r="F230" s="46"/>
+      <c r="G230" s="46"/>
+      <c r="H230" s="46"/>
+      <c r="I230" s="46"/>
+      <c r="J230" s="46"/>
+      <c r="K230" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="39">

</xml_diff>

<commit_message>
Mark ROM WH (erroneously) as a medium carrier.
</commit_message>
<xml_diff>
--- a/sits/msit_rom.xlsx
+++ b/sits/msit_rom.xlsx
@@ -2502,7 +2502,7 @@
     <t>For WE/SK: 6+5</t>
   </si>
   <si>
-    <t>Carrier (Special Type)</t>
+    <t>Carrier (Special Type) Medium Carrier</t>
   </si>
   <si>
     <t>BHF</t>
@@ -4446,8 +4446,8 @@
   </sheetPr>
   <dimension ref="A1:K231"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A196" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H202" activeCellId="0" pane="topLeft" sqref="H202"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A130" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="K148" activeCellId="0" pane="topLeft" sqref="K148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>